<commit_message>
fin TRS y formato
</commit_message>
<xml_diff>
--- a/Riesgo crediticio/22.- TRS.xlsx
+++ b/Riesgo crediticio/22.- TRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolozoya/Documents/ITESO/Semestre 6/Administración de riesgos/Riesgo crediticio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF848F48-D4D4-284A-9B6A-02D9B274B785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9AB799-E12F-4849-9801-99BA6271E720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="3" xr2:uid="{406D6790-6DA7-2D49-A8A7-6AA6B02AC57D}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{406D6790-6DA7-2D49-A8A7-6AA6B02AC57D}"/>
   </bookViews>
   <sheets>
     <sheet name="Teoría" sheetId="1" r:id="rId1"/>
@@ -2367,8 +2367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFD364E-BD99-F245-B75A-DF95DE21BC8C}">
   <dimension ref="B18:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2915,7 +2915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80682B61-D402-3E43-9310-24BA2F087960}">
   <dimension ref="B22:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>

</xml_diff>